<commit_message>
Pull request #21: CNNO-2010 Update HEADERS for file output
Merge in MSFT/microsoft-reports from ~ACELIS/microsoft-reports:bugfix/CNNO-2010-confusing-titles-in-the-audit-tool-reports to master

Squashed commit of the following:

commit 5e92b69399ba7b0bf1838d9454bc15261441543e
Author: Adrian Celis <adrian.celis@cloudblue.com>
Date:   Thu Jan 4 17:33:26 2024 +0100

    CNNO-2010 Update HEADERS for file output
</commit_message>
<xml_diff>
--- a/reports/audit_tool/templates/xlsx/template.xlsx
+++ b/reports/audit_tool/templates/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acelis00\Documents\PythonProjects\adrian-microsoft-reports\reports\audit_tool\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D005A103-0292-4C8D-B486-8422F6871824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31153DA5-2147-4427-BB82-ECA15FD36A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>Transaction Type</t>
   </si>
   <si>
-    <t>CBC Creation Date</t>
-  </si>
-  <si>
     <t>Microsoft Creation Date</t>
   </si>
   <si>
@@ -55,12 +52,6 @@
     <t>Provider ID</t>
   </si>
   <si>
-    <t>CBC Subscription ID</t>
-  </si>
-  <si>
-    <t>CBC Customer ID</t>
-  </si>
-  <si>
     <t>Domain</t>
   </si>
   <si>
@@ -70,22 +61,31 @@
     <t>Offer Name</t>
   </si>
   <si>
-    <t>CBC Status</t>
-  </si>
-  <si>
     <t>Microsoft Status</t>
   </si>
   <si>
     <t>Microsoft Auto Renew</t>
   </si>
   <si>
-    <t>CBC Licenses</t>
-  </si>
-  <si>
     <t>Microsoft Licenses</t>
   </si>
   <si>
     <t>Error details</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Creation Date</t>
+  </si>
+  <si>
+    <t>Licenses</t>
+  </si>
+  <si>
+    <t>External Subscription ID</t>
+  </si>
+  <si>
+    <t>External Customer ID</t>
   </si>
 </sst>
 </file>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,8 +445,8 @@
     <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" customWidth="1"/>
     <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" customWidth="1"/>
+    <col min="7" max="7" width="55.42578125" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
@@ -457,13 +457,13 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -472,10 +472,10 @@
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
@@ -484,40 +484,40 @@
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pull request #26: CNNO-2038 Fix issues with licenses in CSP
Merge in MSFT/microsoft-reports from ~ACELIS/microsoft-reports:bugfix/CNNO-2038-audit-tool-ms-csp-active-subscriptions-are-listed-with-0-units to master

Squashed commit of the following:

commit de1007d9b1cbc4d21503f529e9c829696ee06f9e
Author: Adrian Celis <adrian.celis@cloudblue.com>
Date:   Thu Jan 11 11:23:28 2024 +0100

    CNNO-2038 Fix issues with licenses in CSP

commit 88d37d5c05721599dab89d4274b8306c09557b47
Author: Adrian Celis <adrian.celis@cloudblue.com>
Date:   Thu Jan 11 11:22:20 2024 +0100

    CNNO-2038 Fix issues with licenses in CSP

commit e0da7f43da0cba3af74fc79af80ed47ef853c273
Author: Adrian Celis <adrian.celis@cloudblue.com>
Date:   Thu Jan 11 11:08:24 2024 +0100

    CNNO-2038 Fix issues with licenses in CSP
</commit_message>
<xml_diff>
--- a/reports/audit_tool/templates/xlsx/template.xlsx
+++ b/reports/audit_tool/templates/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acelis00\Documents\PythonProjects\adrian-microsoft-reports\reports\audit_tool\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31153DA5-2147-4427-BB82-ECA15FD36A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7C8C7B-9BC5-405A-8F87-149CD29EED7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,12 +34,6 @@
     <t>Provider Name</t>
   </si>
   <si>
-    <t>Marketplace ID</t>
-  </si>
-  <si>
-    <t>Transaction Type</t>
-  </si>
-  <si>
     <t>Microsoft Creation Date</t>
   </si>
   <si>
@@ -86,6 +80,12 @@
   </si>
   <si>
     <t>External Customer ID</t>
+  </si>
+  <si>
+    <t>Connection Type</t>
+  </si>
+  <si>
+    <t>Marketplace Name</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,67 +457,67 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>